<commit_message>
Update IP - EX 14 - Travamento de celulas (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 14 - Travamento de celulas (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 14 - Travamento de celulas (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C103C4E6-3217-45CC-95A7-E39500B2A59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFB869D-B1C3-4EB5-ACC0-3ED40C4E5455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1004,21 +1004,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dotted">
-        <color theme="1" tint="0.499984740745262"/>
-      </left>
-      <right style="medium">
-        <color theme="1" tint="0.499984740745262"/>
-      </right>
-      <top style="dotted">
-        <color theme="1" tint="0.499984740745262"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="1" tint="0.499984740745262"/>
       </left>
@@ -1060,7 +1045,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1150,16 +1135,10 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1177,7 +1156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2442,103 +2421,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="77"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="75"/>
     </row>
     <row r="3" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="80"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="78"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="78"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="80"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="78"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="78"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="79"/>
-      <c r="Q5" s="80"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="78"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="81"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="83"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="81"/>
     </row>
     <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2562,24 +2541,24 @@
       <c r="Q8" s="23"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="85"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="85"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="86"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+      <c r="M9" s="83"/>
+      <c r="N9" s="83"/>
+      <c r="O9" s="83"/>
+      <c r="P9" s="83"/>
+      <c r="Q9" s="84"/>
     </row>
     <row r="10" spans="2:17" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -2634,18 +2613,18 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="89"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="87"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="90"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="92"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="90"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -2670,35 +2649,35 @@
       <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="L5" s="93" t="s">
+      <c r="L5" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="94"/>
+      <c r="M5" s="92"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="L6" s="95"/>
-      <c r="M6" s="96"/>
+      <c r="L6" s="93"/>
+      <c r="M6" s="94"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="C7" s="2">
         <v>3</v>
       </c>
-      <c r="L7" s="95"/>
-      <c r="M7" s="96"/>
+      <c r="L7" s="93"/>
+      <c r="M7" s="94"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
-      <c r="L8" s="97"/>
-      <c r="M8" s="98"/>
+      <c r="L8" s="95"/>
+      <c r="M8" s="96"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="61" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2724,10 +2703,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="C14" s="62" t="s">
+      <c r="C14" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="62" t="s">
+      <c r="I14" s="60" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2749,18 +2728,18 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="89"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="87"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="90"/>
-      <c r="C18" s="91"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="92"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="90"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
@@ -2777,10 +2756,10 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="C20" s="10"/>
-      <c r="L20" s="93" t="s">
+      <c r="L20" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="M20" s="94"/>
+      <c r="M20" s="92"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
@@ -2793,24 +2772,24 @@
       <c r="E21" s="2">
         <v>3</v>
       </c>
-      <c r="L21" s="95"/>
-      <c r="M21" s="96"/>
+      <c r="L21" s="93"/>
+      <c r="M21" s="94"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="C22" s="13">
         <v>2</v>
       </c>
-      <c r="L22" s="95"/>
-      <c r="M22" s="96"/>
+      <c r="L22" s="93"/>
+      <c r="M22" s="94"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="C23" s="13">
         <v>3</v>
       </c>
-      <c r="L23" s="97"/>
-      <c r="M23" s="98"/>
+      <c r="L23" s="95"/>
+      <c r="M23" s="96"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
@@ -2844,10 +2823,10 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="C31" s="62" t="s">
+      <c r="C31" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="I31" s="62" t="s">
+      <c r="I31" s="60" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2869,18 +2848,18 @@
     </row>
     <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="87" t="s">
+      <c r="B35" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="88"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="89"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="87"/>
     </row>
     <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="90"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="91"/>
-      <c r="E36" s="92"/>
+      <c r="B36" s="88"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="90"/>
     </row>
     <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
@@ -2896,10 +2875,10 @@
     </row>
     <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
-      <c r="L38" s="93" t="s">
+      <c r="L38" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="M38" s="94"/>
+      <c r="M38" s="92"/>
     </row>
     <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
@@ -2914,24 +2893,24 @@
         <v>3</v>
       </c>
       <c r="F39" s="14"/>
-      <c r="L39" s="95"/>
-      <c r="M39" s="96"/>
+      <c r="L39" s="93"/>
+      <c r="M39" s="94"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="C40" s="18">
         <v>2</v>
       </c>
-      <c r="L40" s="95"/>
-      <c r="M40" s="96"/>
+      <c r="L40" s="93"/>
+      <c r="M40" s="94"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="C41" s="2">
         <v>3</v>
       </c>
-      <c r="L41" s="97"/>
-      <c r="M41" s="98"/>
+      <c r="L41" s="95"/>
+      <c r="M41" s="96"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
@@ -2964,10 +2943,10 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
-      <c r="C49" s="62" t="s">
+      <c r="C49" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="I49" s="62" t="s">
+      <c r="I49" s="60" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2989,18 +2968,18 @@
     </row>
     <row r="52" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B53" s="87" t="s">
+      <c r="B53" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="88"/>
-      <c r="D53" s="88"/>
-      <c r="E53" s="89"/>
+      <c r="C53" s="86"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="87"/>
     </row>
     <row r="54" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="90"/>
-      <c r="C54" s="91"/>
-      <c r="D54" s="91"/>
-      <c r="E54" s="92"/>
+      <c r="B54" s="88"/>
+      <c r="C54" s="89"/>
+      <c r="D54" s="89"/>
+      <c r="E54" s="90"/>
     </row>
     <row r="55" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
@@ -3017,10 +2996,10 @@
     <row r="56" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="C56" s="10"/>
-      <c r="L56" s="93" t="s">
+      <c r="L56" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="M56" s="94"/>
+      <c r="M56" s="92"/>
     </row>
     <row r="57" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
@@ -3035,24 +3014,24 @@
         <v>3</v>
       </c>
       <c r="F57" s="14"/>
-      <c r="L57" s="95"/>
-      <c r="M57" s="96"/>
+      <c r="L57" s="93"/>
+      <c r="M57" s="94"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="C58" s="20">
         <v>2</v>
       </c>
-      <c r="L58" s="95"/>
-      <c r="M58" s="96"/>
+      <c r="L58" s="93"/>
+      <c r="M58" s="94"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="C59" s="13">
         <v>3</v>
       </c>
-      <c r="L59" s="97"/>
-      <c r="M59" s="98"/>
+      <c r="L59" s="95"/>
+      <c r="M59" s="96"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
@@ -3086,10 +3065,10 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
-      <c r="C67" s="62" t="s">
+      <c r="C67" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="I67" s="62" t="s">
+      <c r="I67" s="60" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3129,8 +3108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:O47"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3147,94 +3126,94 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="77"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="75"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="80"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="78"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="78"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="80"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="78"/>
     </row>
     <row r="5" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="78"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="80"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="78"/>
     </row>
     <row r="6" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="81"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="83"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="81"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="72" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F9" s="63" t="s">
+      <c r="F9" s="61" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3248,17 +3227,17 @@
       <c r="D10" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="59" t="s">
+      <c r="F10" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="59" t="s">
+      <c r="H10" s="57" t="s">
         <v>7</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="61" t="s">
+      <c r="J10" s="59" t="s">
         <v>34</v>
       </c>
       <c r="K10" s="1"/>
@@ -3271,11 +3250,23 @@
       <c r="C11" s="53">
         <v>87</v>
       </c>
-      <c r="D11" s="56"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="J11" s="64">
+      <c r="D11" s="56">
+        <f>C11*(1-$J$11)</f>
+        <v>73.95</v>
+      </c>
+      <c r="F11" s="58" t="str">
+        <f>IF($B11=F$10,"X","")</f>
+        <v>X</v>
+      </c>
+      <c r="G11" s="58" t="str">
+        <f t="shared" ref="G11:H26" si="0">IF($B11=G$10,"X","")</f>
+        <v/>
+      </c>
+      <c r="H11" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J11" s="62">
         <v>0.15</v>
       </c>
     </row>
@@ -3286,10 +3277,22 @@
       <c r="C12" s="53">
         <v>145</v>
       </c>
-      <c r="D12" s="57"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
+      <c r="D12" s="56">
+        <f t="shared" ref="D12:D30" si="1">C12*(1-$J$11)</f>
+        <v>123.25</v>
+      </c>
+      <c r="F12" s="58" t="str">
+        <f t="shared" ref="F12:H30" si="2">IF($B12=F$10,"X","")</f>
+        <v>X</v>
+      </c>
+      <c r="G12" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H12" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="52" t="s">
@@ -3298,10 +3301,22 @@
       <c r="C13" s="53">
         <v>154</v>
       </c>
-      <c r="D13" s="57"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
+      <c r="D13" s="56">
+        <f t="shared" si="1"/>
+        <v>130.9</v>
+      </c>
+      <c r="F13" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G13" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>X</v>
+      </c>
+      <c r="H13" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="52" t="s">
@@ -3310,10 +3325,22 @@
       <c r="C14" s="53">
         <v>36</v>
       </c>
-      <c r="D14" s="57"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
+      <c r="D14" s="56">
+        <f t="shared" si="1"/>
+        <v>30.599999999999998</v>
+      </c>
+      <c r="F14" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G14" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H14" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>X</v>
+      </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="52" t="s">
@@ -3322,10 +3349,22 @@
       <c r="C15" s="53">
         <v>42</v>
       </c>
-      <c r="D15" s="57"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
+      <c r="D15" s="56">
+        <f t="shared" si="1"/>
+        <v>35.699999999999996</v>
+      </c>
+      <c r="F15" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="G15" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H15" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="52" t="s">
@@ -3334,10 +3373,22 @@
       <c r="C16" s="53">
         <v>44</v>
       </c>
-      <c r="D16" s="57"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
+      <c r="D16" s="56">
+        <f t="shared" si="1"/>
+        <v>37.4</v>
+      </c>
+      <c r="F16" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G16" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H16" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="52" t="s">
@@ -3346,10 +3397,22 @@
       <c r="C17" s="53">
         <v>168</v>
       </c>
-      <c r="D17" s="57"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
+      <c r="D17" s="56">
+        <f t="shared" si="1"/>
+        <v>142.79999999999998</v>
+      </c>
+      <c r="F17" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="G17" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H17" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="52" t="s">
@@ -3358,10 +3421,22 @@
       <c r="C18" s="53">
         <v>158</v>
       </c>
-      <c r="D18" s="57"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
+      <c r="D18" s="56">
+        <f t="shared" si="1"/>
+        <v>134.29999999999998</v>
+      </c>
+      <c r="F18" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G18" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H18" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="52" t="s">
@@ -3370,10 +3445,22 @@
       <c r="C19" s="53">
         <v>64</v>
       </c>
-      <c r="D19" s="57"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
+      <c r="D19" s="56">
+        <f t="shared" si="1"/>
+        <v>54.4</v>
+      </c>
+      <c r="F19" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G19" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H19" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="52" t="s">
@@ -3382,10 +3469,22 @@
       <c r="C20" s="53">
         <v>116</v>
       </c>
-      <c r="D20" s="57"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
+      <c r="D20" s="56">
+        <f t="shared" si="1"/>
+        <v>98.6</v>
+      </c>
+      <c r="F20" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="G20" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H20" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="52" t="s">
@@ -3394,10 +3493,22 @@
       <c r="C21" s="53">
         <v>129</v>
       </c>
-      <c r="D21" s="57"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
+      <c r="D21" s="56">
+        <f t="shared" si="1"/>
+        <v>109.64999999999999</v>
+      </c>
+      <c r="F21" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G21" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H21" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="52" t="s">
@@ -3406,10 +3517,22 @@
       <c r="C22" s="53">
         <v>159</v>
       </c>
-      <c r="D22" s="57"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="60"/>
+      <c r="D22" s="56">
+        <f t="shared" si="1"/>
+        <v>135.15</v>
+      </c>
+      <c r="F22" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="G22" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H22" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="52" t="s">
@@ -3418,10 +3541,22 @@
       <c r="C23" s="53">
         <v>150</v>
       </c>
-      <c r="D23" s="57"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
+      <c r="D23" s="56">
+        <f t="shared" si="1"/>
+        <v>127.5</v>
+      </c>
+      <c r="F23" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G23" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H23" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="52" t="s">
@@ -3430,10 +3565,22 @@
       <c r="C24" s="53">
         <v>81</v>
       </c>
-      <c r="D24" s="57"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
+      <c r="D24" s="56">
+        <f t="shared" si="1"/>
+        <v>68.849999999999994</v>
+      </c>
+      <c r="F24" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G24" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H24" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="52" t="s">
@@ -3442,10 +3589,22 @@
       <c r="C25" s="53">
         <v>100</v>
       </c>
-      <c r="D25" s="57"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
+      <c r="D25" s="56">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="F25" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G25" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H25" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="52" t="s">
@@ -3454,10 +3613,22 @@
       <c r="C26" s="53">
         <v>169</v>
       </c>
-      <c r="D26" s="57"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="60"/>
-      <c r="H26" s="60"/>
+      <c r="D26" s="56">
+        <f t="shared" si="1"/>
+        <v>143.65</v>
+      </c>
+      <c r="F26" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G26" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H26" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="52" t="s">
@@ -3466,10 +3637,22 @@
       <c r="C27" s="53">
         <v>99</v>
       </c>
-      <c r="D27" s="57"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="60"/>
+      <c r="D27" s="56">
+        <f t="shared" si="1"/>
+        <v>84.149999999999991</v>
+      </c>
+      <c r="F27" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G27" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H27" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="52" t="s">
@@ -3478,10 +3661,22 @@
       <c r="C28" s="53">
         <v>54</v>
       </c>
-      <c r="D28" s="57"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
+      <c r="D28" s="56">
+        <f t="shared" si="1"/>
+        <v>45.9</v>
+      </c>
+      <c r="F28" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G28" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H28" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="52" t="s">
@@ -3490,10 +3685,22 @@
       <c r="C29" s="53">
         <v>38</v>
       </c>
-      <c r="D29" s="57"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
+      <c r="D29" s="56">
+        <f t="shared" si="1"/>
+        <v>32.299999999999997</v>
+      </c>
+      <c r="F29" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G29" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H29" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="54" t="s">
@@ -3502,125 +3709,149 @@
       <c r="C30" s="55">
         <v>136</v>
       </c>
-      <c r="D30" s="58"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
+      <c r="D30" s="56">
+        <f t="shared" si="1"/>
+        <v>115.6</v>
+      </c>
+      <c r="F30" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G30" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H30" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
     </row>
     <row r="33" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G33" s="99" t="s">
+      <c r="G33" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="H33" s="99" t="s">
+      <c r="H33" s="97" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="70" t="s">
+      <c r="B34" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="71" t="s">
+      <c r="F34" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="G34" s="99"/>
-      <c r="H34" s="99"/>
+      <c r="G34" s="97"/>
+      <c r="H34" s="97"/>
     </row>
     <row r="35" spans="2:9" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F35" s="72"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="73"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="71"/>
     </row>
     <row r="36" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="67">
+      <c r="B36" s="65">
         <v>14</v>
       </c>
       <c r="D36" s="3"/>
-      <c r="F36" s="69" t="s">
+      <c r="F36" s="67" t="s">
         <v>6</v>
       </c>
       <c r="G36" s="3">
         <v>34</v>
       </c>
-      <c r="H36" s="66"/>
+      <c r="H36" s="64">
+        <f>SUM($B$36:$B$47,G36)</f>
+        <v>251</v>
+      </c>
     </row>
     <row r="37" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="68">
+      <c r="B37" s="66">
         <v>18</v>
       </c>
-      <c r="F37" s="69" t="s">
+      <c r="F37" s="67" t="s">
         <v>19</v>
       </c>
       <c r="G37" s="3">
         <v>23</v>
       </c>
-      <c r="H37" s="66"/>
+      <c r="H37" s="64">
+        <f t="shared" ref="H37:H39" si="3">SUM($B$36:$B$47,G37)</f>
+        <v>240</v>
+      </c>
     </row>
     <row r="38" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="68">
+      <c r="B38" s="66">
         <v>20</v>
       </c>
-      <c r="F38" s="69" t="s">
+      <c r="F38" s="67" t="s">
         <v>1</v>
       </c>
       <c r="G38" s="3">
         <v>11</v>
       </c>
-      <c r="H38" s="66"/>
+      <c r="H38" s="64">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="68">
+      <c r="B39" s="66">
         <v>17</v>
       </c>
-      <c r="F39" s="69" t="s">
+      <c r="F39" s="67" t="s">
         <v>2</v>
       </c>
       <c r="G39" s="3">
         <v>9</v>
       </c>
-      <c r="H39" s="66"/>
+      <c r="H39" s="64">
+        <f t="shared" si="3"/>
+        <v>226</v>
+      </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="68">
+      <c r="B40" s="66">
         <v>17</v>
       </c>
-      <c r="H40" s="65" t="s">
+      <c r="H40" s="63" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="68">
+      <c r="B41" s="66">
         <v>18</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="68">
+      <c r="B42" s="66">
         <v>18</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="68">
+      <c r="B43" s="66">
         <v>18</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="68">
+      <c r="B44" s="66">
         <v>24</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="68">
+      <c r="B45" s="66">
         <v>14</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="68">
+      <c r="B46" s="66">
         <v>24</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="68">
+      <c r="B47" s="66">
         <v>15</v>
       </c>
     </row>

</xml_diff>